<commit_message>
Created Spike to Test MovieLens data set/s
Ran MovieLens 100K through our engine and precision/recall have a much
better shape than our data as n increases (see MetricsSummary-100K.xlsx
for more details).

Not including a .sql or any MovieLens data files as this is a Spike for
testing purposes only.

Also fixed problem in ItemBasedCF that caused recommendations to only be
created for one neighbourhood size when multiple were requested.
</commit_message>
<xml_diff>
--- a/ItemBasedCF/MetricsSummary.xlsx
+++ b/ItemBasedCF/MetricsSummary.xlsx
@@ -361,11 +361,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998472976"/>
-        <c:axId val="-998478960"/>
+        <c:axId val="-184153632"/>
+        <c:axId val="-184156896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998472976"/>
+        <c:axId val="-184153632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,7 +464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998478960"/>
+        <c:crossAx val="-184156896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -472,7 +472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998478960"/>
+        <c:axId val="-184156896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998472976"/>
+        <c:crossAx val="-184153632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -771,7 +771,7 @@
                   <c:v>1.7304747320061199E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6049004594180499E-2</c:v>
+                  <c:v>1.87442572741193E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.2388973966309199E-2</c:v>
@@ -826,7 +826,7 @@
                   <c:v>4.8656326125744E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.14880508334045E-2</c:v>
+                  <c:v>6.6224182208301603E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.6685375417033101E-2</c:v>
@@ -845,11 +845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998486576"/>
-        <c:axId val="-998472432"/>
+        <c:axId val="-184143840"/>
+        <c:axId val="-184146560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998486576"/>
+        <c:axId val="-184143840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998472432"/>
+        <c:crossAx val="-184146560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -956,7 +956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998472432"/>
+        <c:axId val="-184146560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,7 +1007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998486576"/>
+        <c:crossAx val="-184143840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1362,11 +1362,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998481136"/>
-        <c:axId val="-998478416"/>
+        <c:axId val="-184145472"/>
+        <c:axId val="-184144928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998481136"/>
+        <c:axId val="-184145472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,7 +1465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998478416"/>
+        <c:crossAx val="-184144928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1473,7 +1473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998478416"/>
+        <c:axId val="-184144928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1524,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998481136"/>
+        <c:crossAx val="-184145472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,11 +1837,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998480048"/>
-        <c:axId val="-998475152"/>
+        <c:axId val="-184158528"/>
+        <c:axId val="-184157984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998480048"/>
+        <c:axId val="-184158528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998475152"/>
+        <c:crossAx val="-184157984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1948,7 +1948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998475152"/>
+        <c:axId val="-184157984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998480048"/>
+        <c:crossAx val="-184158528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2129,6 +2129,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2317,11 +2318,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998343504"/>
-        <c:axId val="-998346768"/>
+        <c:axId val="-184150912"/>
+        <c:axId val="-316372880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998343504"/>
+        <c:axId val="-184150912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,6 +2354,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2419,7 +2421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998346768"/>
+        <c:crossAx val="-316372880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2427,7 +2429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998346768"/>
+        <c:axId val="-316372880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,7 +2480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998343504"/>
+        <c:crossAx val="-184150912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2608,6 +2610,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2790,11 +2793,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-998348944"/>
-        <c:axId val="-998349488"/>
+        <c:axId val="-178701296"/>
+        <c:axId val="-178702928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998348944"/>
+        <c:axId val="-178701296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2826,6 +2829,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2892,7 +2896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998349488"/>
+        <c:crossAx val="-178702928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2900,7 +2904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998349488"/>
+        <c:axId val="-178702928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-998348944"/>
+        <c:crossAx val="-178701296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6862,7 +6866,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6975,7 +6979,7 @@
         <v>1.7304747320061199E-2</v>
       </c>
       <c r="F7">
-        <v>3.6049004594180499E-2</v>
+        <v>1.87442572741193E-2</v>
       </c>
       <c r="G7">
         <v>2.2388973966309199E-2</v>
@@ -7001,7 +7005,7 @@
         <v>4.8656326125744E-3</v>
       </c>
       <c r="F8">
-        <v>1.14880508334045E-2</v>
+        <v>6.6224182208301603E-3</v>
       </c>
       <c r="G8">
         <v>1.6685375417033101E-2</v>

</xml_diff>